<commit_message>
add new arch v2
add new arch v2. Accracy=0.8421
</commit_message>
<xml_diff>
--- a/results/net_evolution.xlsx
+++ b/results/net_evolution.xlsx
@@ -1,18 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28615"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{329E51AC-1BEC-45A9-9104-15ECB9644B77}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mingjie/Desktop/traffic_signal_classification_task/results/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-3720" yWindow="1740" windowWidth="20740" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -26,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Network changes (starting from the teacher's model)</t>
   </si>
@@ -77,14 +87,20 @@
   </si>
   <si>
     <t>start_epochs_50</t>
+  </si>
+  <si>
+    <t>the number of first layer change from 8 to 16, Dropout from 0.2 to 0.15, epochs fromm 100 to 70</t>
+  </si>
+  <si>
+    <t>new_arch_v2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -124,11 +140,11 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="168" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -405,22 +421,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="122.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="3"/>
+    <col min="1" max="1" width="122.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -455,7 +471,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -469,7 +485,7 @@
         <v>0.2298</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -498,7 +514,7 @@
         <v>0.2656</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -525,6 +541,23 @@
       </c>
       <c r="I4">
         <v>7.2599999999999998E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7">
+        <v>0.84210526332300395</v>
+      </c>
+      <c r="H7">
+        <v>1.4093975310840701</v>
+      </c>
+      <c r="I7">
+        <v>0.31039333343505798</v>
       </c>
     </row>
   </sheetData>

</xml_diff>